<commit_message>
Improved API, documentation, and testing.
</commit_message>
<xml_diff>
--- a/test-resources/excel-files/HomeDepot-CRM-Source build 12.xlsx
+++ b/test-resources/excel-files/HomeDepot-CRM-Source build 12.xlsx
@@ -1213,7 +1213,7 @@
     <t xml:space="preserve">THD-CRM:View customer account page layout</t>
   </si>
   <si>
-    <t xml:space="preserve">THD-CRM:View Order and Line Items of a customer with more than 5 orders</t>
+    <t xml:space="preserve">THD-CRM:Some other made-up test case</t>
   </si>
   <si>
     <t xml:space="preserve">THD-CRM:View STH Fulfillment Order</t>
@@ -1329,14 +1329,14 @@
   </sheetPr>
   <dimension ref="A1:C245"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A236" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B244" activeCellId="0" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="111.99" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="111.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>